<commit_message>
Audit Logs, Holiday Calendar, Company logo and other bug fixes
</commit_message>
<xml_diff>
--- a/Feature Development/EmployeeData_FromShriya.xlsx
+++ b/Feature Development/EmployeeData_FromShriya.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jatink\My_AI_Projects\LMS_v2\Feature Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015717E3-F531-41E6-9F4E-9172BA63EC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E9E5BB-0967-4E86-8DC4-CC0AC9D36F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2032,13 +2032,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="L87" sqref="L87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2112,7 +2113,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
@@ -2160,7 +2161,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
@@ -2208,7 +2209,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
@@ -2256,7 +2257,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>38</v>
       </c>
@@ -2304,7 +2305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
@@ -2352,7 +2353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -2400,7 +2401,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -2448,7 +2449,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
@@ -2496,7 +2497,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>44</v>
       </c>
@@ -2544,7 +2545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>46</v>
       </c>
@@ -2592,7 +2593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>47</v>
       </c>
@@ -2640,7 +2641,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>48</v>
       </c>
@@ -2688,7 +2689,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>49</v>
       </c>
@@ -2736,7 +2737,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>50</v>
       </c>
@@ -2784,7 +2785,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>52</v>
       </c>
@@ -2832,7 +2833,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>53</v>
       </c>
@@ -2880,7 +2881,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>54</v>
       </c>
@@ -2928,7 +2929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>55</v>
       </c>
@@ -2976,7 +2977,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
@@ -3024,7 +3025,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>57</v>
       </c>
@@ -3072,7 +3073,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>58</v>
       </c>
@@ -3120,7 +3121,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>59</v>
       </c>
@@ -3168,7 +3169,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>60</v>
       </c>
@@ -3216,7 +3217,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>61</v>
       </c>
@@ -3264,7 +3265,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>62</v>
       </c>
@@ -3312,7 +3313,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>63</v>
       </c>
@@ -3360,7 +3361,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>65</v>
       </c>
@@ -3408,7 +3409,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>66</v>
       </c>
@@ -3456,7 +3457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>67</v>
       </c>
@@ -3504,7 +3505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>68</v>
       </c>
@@ -3552,7 +3553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>69</v>
       </c>
@@ -3600,7 +3601,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>70</v>
       </c>
@@ -3648,7 +3649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>72</v>
       </c>
@@ -3696,7 +3697,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>73</v>
       </c>
@@ -3744,7 +3745,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>74</v>
       </c>
@@ -3792,7 +3793,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>75</v>
       </c>
@@ -3840,7 +3841,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>76</v>
       </c>
@@ -3888,7 +3889,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>77</v>
       </c>
@@ -3936,7 +3937,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>78</v>
       </c>
@@ -3984,7 +3985,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>79</v>
       </c>
@@ -4032,7 +4033,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>80</v>
       </c>
@@ -4080,7 +4081,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>81</v>
       </c>
@@ -4128,7 +4129,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>82</v>
       </c>
@@ -4176,7 +4177,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>83</v>
       </c>
@@ -4224,7 +4225,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>84</v>
       </c>
@@ -4272,7 +4273,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>85</v>
       </c>
@@ -4320,7 +4321,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>86</v>
       </c>
@@ -4368,7 +4369,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>87</v>
       </c>
@@ -4416,7 +4417,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>88</v>
       </c>
@@ -4464,7 +4465,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>89</v>
       </c>
@@ -4512,7 +4513,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>90</v>
       </c>
@@ -4560,7 +4561,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>91</v>
       </c>
@@ -4608,7 +4609,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>92</v>
       </c>
@@ -4656,7 +4657,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>93</v>
       </c>
@@ -4704,7 +4705,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>94</v>
       </c>
@@ -4752,7 +4753,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>95</v>
       </c>
@@ -4800,7 +4801,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>96</v>
       </c>
@@ -4848,7 +4849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>97</v>
       </c>
@@ -4896,7 +4897,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>99</v>
       </c>
@@ -4944,7 +4945,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>100</v>
       </c>
@@ -4992,7 +4993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>101</v>
       </c>
@@ -5040,7 +5041,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>103</v>
       </c>
@@ -5088,7 +5089,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>104</v>
       </c>
@@ -5136,7 +5137,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>106</v>
       </c>
@@ -5184,7 +5185,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>107</v>
       </c>
@@ -5232,7 +5233,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>108</v>
       </c>
@@ -5280,7 +5281,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>109</v>
       </c>
@@ -5328,7 +5329,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>111</v>
       </c>
@@ -5376,7 +5377,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>112</v>
       </c>
@@ -5424,7 +5425,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>113</v>
       </c>
@@ -5472,7 +5473,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>114</v>
       </c>
@@ -5520,7 +5521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>115</v>
       </c>
@@ -5568,7 +5569,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>116</v>
       </c>
@@ -5616,7 +5617,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>118</v>
       </c>
@@ -5664,7 +5665,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>119</v>
       </c>
@@ -5712,7 +5713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>120</v>
       </c>
@@ -5760,7 +5761,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>121</v>
       </c>
@@ -5808,7 +5809,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>122</v>
       </c>
@@ -5856,7 +5857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>123</v>
       </c>
@@ -5904,7 +5905,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>124</v>
       </c>
@@ -5952,7 +5953,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>125</v>
       </c>
@@ -6000,7 +6001,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>126</v>
       </c>
@@ -6048,7 +6049,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>272</v>
       </c>
@@ -6096,7 +6097,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>127</v>
       </c>
@@ -6240,7 +6241,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>273</v>
       </c>
@@ -6288,7 +6289,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>130</v>
       </c>
@@ -6528,7 +6529,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>135</v>
       </c>
@@ -6576,7 +6577,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>325</v>
       </c>
@@ -6624,7 +6625,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>278</v>
       </c>
@@ -6672,7 +6673,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>279</v>
       </c>
@@ -6720,7 +6721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>280</v>
       </c>
@@ -6768,7 +6769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>281</v>
       </c>
@@ -6816,7 +6817,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>282</v>
       </c>
@@ -6864,7 +6865,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>283</v>
       </c>
@@ -6912,7 +6913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>284</v>
       </c>
@@ -6960,7 +6961,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>285</v>
       </c>
@@ -7006,7 +7007,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>286</v>
       </c>
@@ -7054,7 +7055,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>178</v>
       </c>
@@ -7102,7 +7103,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>287</v>
       </c>
@@ -7150,7 +7151,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>288</v>
       </c>
@@ -7295,7 +7296,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P109" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:P109" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="Consultant"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E16" r:id="rId1" display="mailto:rupeshn@golivefaster.com" xr:uid="{BF8D776C-3BF0-4D57-8E6E-EE2174FEC82A}"/>

</xml_diff>

<commit_message>
Data Cleanup, LMS user creation bug fix, leave balances sql script
</commit_message>
<xml_diff>
--- a/Feature Development/EmployeeData_FromShriya.xlsx
+++ b/Feature Development/EmployeeData_FromShriya.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jatink\My_AI_Projects\LMS_v2\Feature Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E9E5BB-0967-4E86-8DC4-CC0AC9D36F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2924BB82-C3F9-4374-B8C6-86D9598E6AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="520">
   <si>
     <t>Employee ID</t>
   </si>
@@ -428,9 +428,6 @@
     <t>T-176</t>
   </si>
   <si>
-    <t>Aparna Godbole</t>
-  </si>
-  <si>
     <t>Z1139</t>
   </si>
   <si>
@@ -846,9 +843,6 @@
   </si>
   <si>
     <t>richa@golivefaster.com</t>
-  </si>
-  <si>
-    <t>9765855570/8956471081</t>
   </si>
   <si>
     <t>Contractor</t>
@@ -2032,14 +2026,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:P109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L87" sqref="L87"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2083,10 +2076,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>4</v>
@@ -2113,21 +2106,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F2" s="7">
         <v>9850540057</v>
@@ -2140,7 +2133,7 @@
         <v>13</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>14</v>
@@ -2149,10 +2142,10 @@
         <v>32</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>16</v>
@@ -2161,21 +2154,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F3" s="7">
         <v>9850489110</v>
@@ -2188,19 +2181,19 @@
         <v>13</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>16</v>
@@ -2209,21 +2202,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F4" s="7">
         <v>8308712376</v>
@@ -2236,10 +2229,10 @@
         <v>13</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>32</v>
@@ -2257,21 +2250,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F5" s="7">
         <v>9822597977</v>
@@ -2284,10 +2277,10 @@
         <v>13</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>32</v>
@@ -2305,21 +2298,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F6" s="7">
         <v>9664341098</v>
@@ -2332,10 +2325,10 @@
         <v>13</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>32</v>
@@ -2353,21 +2346,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F7" s="7">
         <v>9975119845</v>
@@ -2380,7 +2373,7 @@
         <v>13</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>14</v>
@@ -2401,21 +2394,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F8" s="7">
         <v>9657866795</v>
@@ -2428,10 +2421,10 @@
         <v>13</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>32</v>
@@ -2449,21 +2442,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F9" s="7">
         <v>8551835737</v>
@@ -2476,7 +2469,7 @@
         <v>13</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>14</v>
@@ -2497,21 +2490,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F10" s="7">
         <v>9284342804</v>
@@ -2524,7 +2517,7 @@
         <v>13</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>14</v>
@@ -2545,21 +2538,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F11" s="7">
         <v>9657966105</v>
@@ -2572,10 +2565,10 @@
         <v>13</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>32</v>
@@ -2593,21 +2586,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F12" s="7">
         <v>9730317620</v>
@@ -2620,7 +2613,7 @@
         <v>13</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>14</v>
@@ -2641,21 +2634,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F13" s="7">
         <v>9975773902</v>
@@ -2668,10 +2661,10 @@
         <v>13</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>32</v>
@@ -2689,21 +2682,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F14" s="7">
         <v>8087774803</v>
@@ -2716,10 +2709,10 @@
         <v>13</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>32</v>
@@ -2737,21 +2730,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F15" s="7">
         <v>9922993606</v>
@@ -2764,19 +2757,19 @@
         <v>13</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>16</v>
@@ -2785,21 +2778,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F16" s="7">
         <v>9309821711</v>
@@ -2812,7 +2805,7 @@
         <v>13</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>14</v>
@@ -2833,21 +2826,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F17" s="7">
         <v>8668387436</v>
@@ -2860,7 +2853,7 @@
         <v>13</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>14</v>
@@ -2881,7 +2874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>54</v>
       </c>
@@ -2892,7 +2885,7 @@
         <v>27</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>28</v>
@@ -2908,10 +2901,10 @@
         <v>13</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>32</v>
@@ -2929,21 +2922,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F19" s="7">
         <v>7350666250</v>
@@ -2956,7 +2949,7 @@
         <v>13</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>14</v>
@@ -2977,21 +2970,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F20" s="7">
         <v>7028314533</v>
@@ -3004,10 +2997,10 @@
         <v>13</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>32</v>
@@ -3025,21 +3018,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F21" s="7">
         <v>7028926539</v>
@@ -3052,19 +3045,19 @@
         <v>13</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O21" s="5" t="s">
         <v>30</v>
@@ -3073,21 +3066,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F22" s="7">
         <v>9405614270</v>
@@ -3100,7 +3093,7 @@
         <v>13</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>14</v>
@@ -3121,21 +3114,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F23" s="7">
         <v>8459331499</v>
@@ -3148,19 +3141,19 @@
         <v>13</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O23" s="5" t="s">
         <v>30</v>
@@ -3169,21 +3162,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F24" s="7">
         <v>9130795344</v>
@@ -3196,10 +3189,10 @@
         <v>13</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>32</v>
@@ -3217,21 +3210,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F25" s="7">
         <v>8237484013</v>
@@ -3244,19 +3237,19 @@
         <v>13</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O25" s="5" t="s">
         <v>30</v>
@@ -3265,21 +3258,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F26" s="7">
         <v>8980497707</v>
@@ -3292,10 +3285,10 @@
         <v>13</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>32</v>
@@ -3313,7 +3306,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>63</v>
       </c>
@@ -3324,7 +3317,7 @@
         <v>11</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>12</v>
@@ -3340,7 +3333,7 @@
         <v>13</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>14</v>
@@ -3361,21 +3354,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F28" s="7">
         <v>9145242576</v>
@@ -3388,19 +3381,19 @@
         <v>13</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O28" s="5" t="s">
         <v>30</v>
@@ -3409,21 +3402,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F29" s="7">
         <v>7775908621</v>
@@ -3436,7 +3429,7 @@
         <v>13</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>14</v>
@@ -3457,21 +3450,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F30" s="7">
         <v>8275844696</v>
@@ -3484,7 +3477,7 @@
         <v>13</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>14</v>
@@ -3505,21 +3498,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F31" s="7">
         <v>9975525384</v>
@@ -3532,7 +3525,7 @@
         <v>13</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>14</v>
@@ -3553,21 +3546,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F32" s="7">
         <v>8329317675</v>
@@ -3580,19 +3573,19 @@
         <v>13</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O32" s="5" t="s">
         <v>30</v>
@@ -3601,21 +3594,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F33" s="7">
         <v>9881417971</v>
@@ -3628,7 +3621,7 @@
         <v>13</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>14</v>
@@ -3649,21 +3642,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F34" s="7">
         <v>7415403047</v>
@@ -3676,7 +3669,7 @@
         <v>13</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>14</v>
@@ -3697,21 +3690,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F35" s="7">
         <v>9552199200</v>
@@ -3724,7 +3717,7 @@
         <v>13</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>14</v>
@@ -3745,21 +3738,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F36" s="7">
         <v>8080948652</v>
@@ -3772,19 +3765,19 @@
         <v>13</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O36" s="5" t="s">
         <v>30</v>
@@ -3793,21 +3786,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F37" s="7">
         <v>9921213629</v>
@@ -3820,19 +3813,19 @@
         <v>13</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O37" s="5" t="s">
         <v>30</v>
@@ -3841,21 +3834,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F38" s="7">
         <v>9158514389</v>
@@ -3868,7 +3861,7 @@
         <v>13</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>14</v>
@@ -3889,21 +3882,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F39" s="7">
         <v>8180985327</v>
@@ -3916,19 +3909,19 @@
         <v>13</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L39" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O39" s="5" t="s">
         <v>30</v>
@@ -3937,21 +3930,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F40" s="7">
         <v>9623200213</v>
@@ -3964,7 +3957,7 @@
         <v>13</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>14</v>
@@ -3985,24 +3978,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>269</v>
+        <v>216</v>
+      </c>
+      <c r="F41" s="7">
+        <v>9765855570</v>
       </c>
       <c r="G41" s="8">
         <v>44805</v>
@@ -4012,19 +4005,19 @@
         <v>13</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O41" s="5" t="s">
         <v>30</v>
@@ -4033,21 +4026,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>398</v>
-      </c>
       <c r="D42" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F42" s="7">
         <v>8390758247</v>
@@ -4060,19 +4053,19 @@
         <v>13</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L42" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O42" s="5" t="s">
         <v>30</v>
@@ -4081,21 +4074,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F43" s="7">
         <v>8888552986</v>
@@ -4108,7 +4101,7 @@
         <v>13</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>14</v>
@@ -4129,21 +4122,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F44" s="7">
         <v>8788149307</v>
@@ -4156,7 +4149,7 @@
         <v>13</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>14</v>
@@ -4177,21 +4170,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F45" s="7">
         <v>7083836530</v>
@@ -4204,7 +4197,7 @@
         <v>13</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>14</v>
@@ -4213,10 +4206,10 @@
         <v>32</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O45" s="5" t="s">
         <v>30</v>
@@ -4225,21 +4218,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>84</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F46" s="7">
         <v>9822584997</v>
@@ -4252,7 +4245,7 @@
         <v>13</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K46" s="4" t="s">
         <v>14</v>
@@ -4273,21 +4266,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F47" s="7">
         <v>7387786514</v>
@@ -4300,10 +4293,10 @@
         <v>13</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L47" s="4" t="s">
         <v>32</v>
@@ -4321,21 +4314,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>86</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F48" s="7">
         <v>9284826079</v>
@@ -4348,19 +4341,19 @@
         <v>13</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N48" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O48" s="5" t="s">
         <v>30</v>
@@ -4369,21 +4362,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>87</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F49" s="7">
         <v>7721941091</v>
@@ -4396,7 +4389,7 @@
         <v>13</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K49" s="4" t="s">
         <v>14</v>
@@ -4417,21 +4410,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F50" s="7">
         <v>7588252509</v>
@@ -4444,10 +4437,10 @@
         <v>13</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>32</v>
@@ -4465,21 +4458,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F51" s="7">
         <v>8483035819</v>
@@ -4492,10 +4485,10 @@
         <v>13</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>32</v>
@@ -4513,21 +4506,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F52" s="7">
         <v>7776062458</v>
@@ -4540,10 +4533,10 @@
         <v>13</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>32</v>
@@ -4561,21 +4554,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>91</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F53" s="7">
         <v>8308773894</v>
@@ -4588,10 +4581,10 @@
         <v>13</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>32</v>
@@ -4609,21 +4602,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F54" s="7">
         <v>9011691705</v>
@@ -4636,19 +4629,19 @@
         <v>13</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O54" s="5" t="s">
         <v>30</v>
@@ -4657,7 +4650,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>93</v>
       </c>
@@ -4668,7 +4661,7 @@
         <v>19</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>20</v>
@@ -4684,10 +4677,10 @@
         <v>13</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>32</v>
@@ -4705,21 +4698,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>94</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F56" s="7">
         <v>7218529583</v>
@@ -4732,19 +4725,19 @@
         <v>13</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N56" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O56" s="5" t="s">
         <v>30</v>
@@ -4753,21 +4746,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>95</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F57" s="7">
         <v>9009251737</v>
@@ -4780,19 +4773,19 @@
         <v>13</v>
       </c>
       <c r="J57" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L57" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O57" s="5" t="s">
         <v>30</v>
@@ -4801,21 +4794,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>96</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F58" s="7">
         <v>9359896823</v>
@@ -4828,19 +4821,19 @@
         <v>13</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L58" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O58" s="5" t="s">
         <v>30</v>
@@ -4849,21 +4842,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F59" s="4">
         <v>7972565199</v>
@@ -4876,19 +4869,19 @@
         <v>13</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L59" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N59" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O59" s="5" t="s">
         <v>16</v>
@@ -4897,21 +4890,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>99</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F60" s="7">
         <v>9284787598</v>
@@ -4924,10 +4917,10 @@
         <v>13</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L60" s="4" t="s">
         <v>32</v>
@@ -4945,21 +4938,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>100</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F61" s="7">
         <v>8087679900</v>
@@ -4972,10 +4965,10 @@
         <v>13</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L61" s="4" t="s">
         <v>32</v>
@@ -4993,21 +4986,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F62" s="7">
         <v>9766541020</v>
@@ -5020,10 +5013,10 @@
         <v>13</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L62" s="4" t="s">
         <v>32</v>
@@ -5041,21 +5034,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F63" s="7">
         <v>9730895314</v>
@@ -5068,19 +5061,19 @@
         <v>13</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L63" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O63" s="5" t="s">
         <v>30</v>
@@ -5089,21 +5082,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>104</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F64" s="7">
         <v>9922689654</v>
@@ -5116,10 +5109,10 @@
         <v>13</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L64" s="4" t="s">
         <v>32</v>
@@ -5137,21 +5130,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>106</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F65" s="7">
         <v>9766892861</v>
@@ -5164,19 +5157,19 @@
         <v>13</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L65" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="O65" s="5" t="s">
         <v>30</v>
@@ -5185,21 +5178,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F66" s="10">
         <v>9930488269</v>
@@ -5212,19 +5205,19 @@
         <v>13</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L66" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N66" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O66" s="5" t="s">
         <v>30</v>
@@ -5233,21 +5226,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>108</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F67" s="7">
         <v>9763789714</v>
@@ -5260,19 +5253,19 @@
         <v>13</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L67" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N67" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O67" s="5" t="s">
         <v>30</v>
@@ -5281,21 +5274,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F68" s="7">
         <v>7721960088</v>
@@ -5308,10 +5301,10 @@
         <v>13</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K68" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L68" s="4" t="s">
         <v>32</v>
@@ -5329,21 +5322,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>111</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F69" s="7">
         <v>9860165063</v>
@@ -5356,10 +5349,10 @@
         <v>13</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K69" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L69" s="4" t="s">
         <v>32</v>
@@ -5377,21 +5370,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F70" s="7">
         <v>7587292703</v>
@@ -5404,7 +5397,7 @@
         <v>13</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K70" s="4" t="s">
         <v>14</v>
@@ -5425,21 +5418,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F71" s="7">
         <v>9518768204</v>
@@ -5452,10 +5445,10 @@
         <v>13</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L71" s="4" t="s">
         <v>32</v>
@@ -5473,21 +5466,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F72" s="7">
         <v>9766695894</v>
@@ -5500,19 +5493,19 @@
         <v>13</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K72" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L72" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O72" s="5" t="s">
         <v>30</v>
@@ -5521,21 +5514,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F73" s="7">
         <v>8688257031</v>
@@ -5548,19 +5541,19 @@
         <v>13</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K73" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L73" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N73" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O73" s="5" t="s">
         <v>30</v>
@@ -5569,21 +5562,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>116</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F74" s="7">
         <v>9404608989</v>
@@ -5596,7 +5589,7 @@
         <v>13</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K74" s="4" t="s">
         <v>14</v>
@@ -5617,21 +5610,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F75" s="7">
         <v>7038868314</v>
@@ -5644,19 +5637,19 @@
         <v>13</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K75" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L75" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N75" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O75" s="5" t="s">
         <v>30</v>
@@ -5665,21 +5658,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F76" s="4">
         <v>9767815119</v>
@@ -5692,10 +5685,10 @@
         <v>13</v>
       </c>
       <c r="J76" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K76" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L76" s="4" t="s">
         <v>32</v>
@@ -5713,21 +5706,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F77" s="7">
         <v>9623481211</v>
@@ -5740,10 +5733,10 @@
         <v>13</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K77" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L77" s="4" t="s">
         <v>32</v>
@@ -5761,21 +5754,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F78" s="7">
         <v>8329302306</v>
@@ -5788,19 +5781,19 @@
         <v>13</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K78" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L78" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N78" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O78" s="5" t="s">
         <v>30</v>
@@ -5809,21 +5802,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>122</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F79" s="7">
         <v>9623713881</v>
@@ -5836,19 +5829,19 @@
         <v>13</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K79" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L79" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M79" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N79" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O79" s="5" t="s">
         <v>30</v>
@@ -5857,21 +5850,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>123</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F80" s="4">
         <v>9527046204</v>
@@ -5884,19 +5877,19 @@
         <v>13</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K80" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L80" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M80" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O80" s="5" t="s">
         <v>30</v>
@@ -5905,21 +5898,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>124</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F81" s="7">
         <v>9607153545</v>
@@ -5932,7 +5925,7 @@
         <v>13</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K81" s="4" t="s">
         <v>14</v>
@@ -5953,21 +5946,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>125</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F82" s="7">
         <v>8830596215</v>
@@ -5980,19 +5973,19 @@
         <v>13</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K82" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L82" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M82" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O82" s="5" t="s">
         <v>30</v>
@@ -6001,21 +5994,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>126</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F83" s="7">
         <v>7869917622</v>
@@ -6028,19 +6021,19 @@
         <v>13</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K83" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L83" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M83" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N83" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="O83" s="5" t="s">
         <v>30</v>
@@ -6049,21 +6042,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F84" s="7">
         <v>7066167700</v>
@@ -6076,19 +6069,19 @@
         <v>13</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K84" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L84" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="M84" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N84" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O84" s="5" t="s">
         <v>30</v>
@@ -6097,7 +6090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>127</v>
       </c>
@@ -6108,7 +6101,7 @@
         <v>22</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>23</v>
@@ -6124,13 +6117,13 @@
         <v>13</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>14</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="M85" s="4" t="s">
         <v>24</v>
@@ -6150,16 +6143,16 @@
         <v>128</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F86" s="7">
         <v>9970967541</v>
@@ -6172,13 +6165,13 @@
         <v>13</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K86" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L86" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M86" s="4" t="s">
         <v>105</v>
@@ -6195,19 +6188,19 @@
     </row>
     <row r="87" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F87" s="7">
         <v>9326092957</v>
@@ -6220,13 +6213,13 @@
         <v>13</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K87" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="L87" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M87" s="4" t="s">
         <v>24</v>
@@ -6241,21 +6234,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F88" s="7">
         <v>9980921464</v>
@@ -6268,13 +6261,13 @@
         <v>13</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K88" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L88" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="M88" s="4" t="s">
         <v>15</v>
@@ -6289,21 +6282,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F89" s="7">
         <v>8551906351</v>
@@ -6316,7 +6309,7 @@
         <v>13</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K89" s="4" t="s">
         <v>14</v>
@@ -6339,19 +6332,19 @@
     </row>
     <row r="90" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F90" s="7">
         <v>8668775175</v>
@@ -6364,13 +6357,13 @@
         <v>13</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K90" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L90" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M90" s="4" t="s">
         <v>105</v>
@@ -6387,19 +6380,19 @@
     </row>
     <row r="91" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F91" s="7">
         <v>9420891124</v>
@@ -6412,13 +6405,13 @@
         <v>13</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K91" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L91" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M91" s="4" t="s">
         <v>40</v>
@@ -6435,19 +6428,19 @@
     </row>
     <row r="92" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F92" s="7">
         <v>7218444115</v>
@@ -6460,19 +6453,19 @@
         <v>13</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K92" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L92" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M92" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N92" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O92" s="5" t="s">
         <v>30</v>
@@ -6483,19 +6476,19 @@
     </row>
     <row r="93" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F93" s="7">
         <v>9699859895</v>
@@ -6508,19 +6501,19 @@
         <v>13</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K93" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L93" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M93" s="4" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="N93" s="4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O93" s="5" t="s">
         <v>30</v>
@@ -6529,21 +6522,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F94" s="7">
         <v>9766311359</v>
@@ -6556,13 +6549,13 @@
         <v>13</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K94" s="4" t="s">
         <v>14</v>
       </c>
       <c r="L94" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="M94" s="4" t="s">
         <v>64</v>
@@ -6577,21 +6570,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F95" s="12">
         <v>9132069430</v>
@@ -6601,13 +6594,13 @@
       </c>
       <c r="H95" s="8"/>
       <c r="I95" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K95" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L95" s="4" t="s">
         <v>32</v>
@@ -6625,21 +6618,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F96" s="7">
         <v>9377070170</v>
@@ -6649,22 +6642,22 @@
       </c>
       <c r="H96" s="8"/>
       <c r="I96" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K96" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L96" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M96" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N96" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O96" s="5" t="s">
         <v>30</v>
@@ -6673,34 +6666,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G97" s="8">
         <v>44467</v>
       </c>
       <c r="H97" s="8"/>
       <c r="I97" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K97" s="4" t="s">
         <v>14</v>
@@ -6721,34 +6714,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F98" s="12" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="G98" s="8">
         <v>44501</v>
       </c>
       <c r="H98" s="8"/>
       <c r="I98" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K98" s="4" t="s">
         <v>14</v>
@@ -6769,34 +6762,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G99" s="8">
         <v>44566</v>
       </c>
       <c r="H99" s="8"/>
       <c r="I99" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J99" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K99" s="4" t="s">
         <v>14</v>
@@ -6817,34 +6810,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F100" s="12" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="G100" s="8">
         <v>44651</v>
       </c>
       <c r="H100" s="8"/>
       <c r="I100" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K100" s="4" t="s">
         <v>14</v>
@@ -6865,21 +6858,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F101" s="7">
         <v>9914459122</v>
@@ -6889,16 +6882,16 @@
       </c>
       <c r="H101" s="8"/>
       <c r="I101" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J101" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K101" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L101" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="M101" s="4" t="s">
         <v>24</v>
@@ -6913,34 +6906,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G102" s="8">
         <v>45614</v>
       </c>
       <c r="H102" s="8"/>
       <c r="I102" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J102" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K102" s="4" t="s">
         <v>14</v>
@@ -6961,21 +6954,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F103" s="7"/>
       <c r="G103" s="8">
@@ -6983,10 +6976,10 @@
       </c>
       <c r="H103" s="8"/>
       <c r="I103" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J103" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K103" s="4" t="s">
         <v>14</v>
@@ -7007,37 +7000,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F104" s="12" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="G104" s="8">
         <v>45719</v>
       </c>
       <c r="H104" s="8"/>
       <c r="I104" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J104" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K104" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="L104" s="4" t="s">
         <v>32</v>
@@ -7055,21 +7048,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B105" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="D105" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="C105" s="5" t="s">
-        <v>501</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>512</v>
-      </c>
       <c r="E105" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F105" s="7">
         <v>9421673527</v>
@@ -7079,16 +7072,16 @@
       </c>
       <c r="H105" s="8"/>
       <c r="I105" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J105" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K105" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L105" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="M105" s="4" t="s">
         <v>105</v>
@@ -7103,37 +7096,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G106" s="8">
         <v>45819</v>
       </c>
       <c r="H106" s="8"/>
       <c r="I106" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J106" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K106" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="L106" s="4" t="s">
         <v>32</v>
@@ -7151,37 +7144,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G107" s="8">
         <v>45859</v>
       </c>
       <c r="H107" s="8"/>
       <c r="I107" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J107" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="K107" s="4" t="s">
         <v>300</v>
-      </c>
-      <c r="K107" s="4" t="s">
-        <v>302</v>
       </c>
       <c r="L107" s="4" t="s">
         <v>32</v>
@@ -7201,19 +7194,19 @@
     </row>
     <row r="108" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D108" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E108" s="14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F108" s="15">
         <v>8563980285</v>
@@ -7223,22 +7216,22 @@
       </c>
       <c r="H108" s="16"/>
       <c r="I108" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J108" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K108" s="13" t="s">
         <v>14</v>
       </c>
       <c r="L108" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M108" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="N108" s="13" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="O108" s="5" t="s">
         <v>30</v>
@@ -7249,38 +7242,38 @@
     </row>
     <row r="109" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D109" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F109" s="17" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="G109" s="16">
         <v>45901</v>
       </c>
       <c r="H109" s="16"/>
       <c r="I109" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J109" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K109" s="4" t="s">
         <v>14</v>
       </c>
       <c r="L109" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M109" s="4" t="s">
         <v>64</v>
@@ -7296,13 +7289,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P109" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="Consultant"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:P109" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E16" r:id="rId1" display="mailto:rupeshn@golivefaster.com" xr:uid="{BF8D776C-3BF0-4D57-8E6E-EE2174FEC82A}"/>

</xml_diff>